<commit_message>
Agregado campo importe a factura y se llena.
</commit_message>
<xml_diff>
--- a/tpGestion.xlsx
+++ b/tpGestion.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="14115" windowHeight="4680"/>
@@ -10,12 +10,12 @@
     <sheet name="Clientes y operaciones" sheetId="1" r:id="rId1"/>
     <sheet name="Roles y usuarios" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="96">
   <si>
     <t>Cliente</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t>x                        x</t>
+  </si>
+  <si>
+    <t>importe</t>
   </si>
 </sst>
 </file>
@@ -331,7 +334,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,6 +353,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -480,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -510,6 +519,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:P34"/>
+  <dimension ref="B1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1620,15 +1632,26 @@
       </c>
       <c r="L33" s="6"/>
     </row>
-    <row r="34" spans="6:12" ht="15.75" thickBot="1">
-      <c r="J34" s="14" t="s">
+    <row r="34" spans="6:12">
+      <c r="J34" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K34" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="L34" s="16" t="s">
+      <c r="K34" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L34" s="6" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="6:12" ht="15.75" thickBot="1">
+      <c r="J35" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="K35" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="L35" s="31" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>